<commit_message>
Updated code for new dataset version, added new sample code
</commit_message>
<xml_diff>
--- a/Conversion/BuildingTypeNames.xlsx
+++ b/Conversion/BuildingTypeNames.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/repos/A-Construction-Classification-System-Database-for-Understanding-Resource-Use-in-Buildings/Conversion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C221A39F-2F9C-804F-8206-84319034899B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C34E28EA-4281-ED4E-A7CB-4F5F5D1DE57B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4700" yWindow="3200" windowWidth="27240" windowHeight="16440" xr2:uid="{8F425863-01D1-854A-BB5C-84F03FFBF593}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{8F425863-01D1-854A-BB5C-84F03FFBF593}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
   <si>
     <t>Building Type</t>
   </si>
@@ -131,16 +131,32 @@
   </si>
   <si>
     <t>SNR</t>
+  </si>
+  <si>
+    <t>TWN</t>
+  </si>
+  <si>
+    <t>Public Facility</t>
+  </si>
+  <si>
+    <t>PUF</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -166,8 +182,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -482,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{546A72BF-51E5-9D49-ADAA-34F0E31097F5}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -495,7 +529,7 @@
     <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -506,150 +540,203 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="D3" s="1"/>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C5" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="D5" s="1"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B8" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C8" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>17</v>
+      <c r="D8" s="1"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
         <v>4</v>
       </c>
-      <c r="C10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C10" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>21</v>
       </c>
       <c r="B11" t="s">
         <v>4</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11" s="1"/>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" t="s">
-        <v>29</v>
-      </c>
+      <c r="B16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="2"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C15">
+    <sortCondition ref="C2:C15"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>